<commit_message>
Updated BGR model - 2025-08-17 18:41
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_BGR/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86862ACB-51DC-4323-9388-188472C23E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC673B1-FB36-42E4-901D-18DD441F412D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVA" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="67">
   <si>
     <t>PSET_PN</t>
   </si>
@@ -112,12 +112,6 @@
     <t>io</t>
   </si>
   <si>
-    <t>ELC_Sol*</t>
-  </si>
-  <si>
-    <t>ELC_Win*</t>
-  </si>
-  <si>
     <t>IN</t>
   </si>
   <si>
@@ -230,6 +224,21 @@
   </si>
   <si>
     <t>allregions</t>
+  </si>
+  <si>
+    <t>ELC_spv*</t>
+  </si>
+  <si>
+    <t>ELC_won*</t>
+  </si>
+  <si>
+    <t>Trd_elec*</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>wind</t>
   </si>
 </sst>
 </file>
@@ -558,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268E9BAB-B98F-4B82-9042-51EABC9ED525}">
   <dimension ref="B3:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -566,7 +575,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -574,12 +583,12 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -617,13 +626,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
@@ -632,69 +641,69 @@
         <v>22</v>
       </c>
       <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>44</v>
-      </c>
-      <c r="N1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2">
         <v>2700</v>
@@ -706,42 +715,42 @@
         <v>2700</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L3">
         <v>1110</v>
@@ -753,42 +762,42 @@
         <v>480</v>
       </c>
       <c r="O3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L4">
         <v>4060</v>
@@ -800,42 +809,42 @@
         <v>1980</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L5">
         <v>1500</v>
@@ -847,42 +856,42 @@
         <v>1370</v>
       </c>
       <c r="O5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
         <v>49</v>
       </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L6">
         <v>70</v>
@@ -894,42 +903,42 @@
         <v>65</v>
       </c>
       <c r="O6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L7">
         <v>16</v>
@@ -941,42 +950,42 @@
         <v>16</v>
       </c>
       <c r="O7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L8">
         <v>120</v>
@@ -988,42 +997,42 @@
         <v>70</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L9">
         <v>38</v>
@@ -1035,42 +1044,42 @@
         <v>36</v>
       </c>
       <c r="O9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -1082,42 +1091,42 @@
         <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L11">
         <v>1.5</v>
@@ -1129,42 +1138,42 @@
         <v>1.5</v>
       </c>
       <c r="O11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L12">
         <v>3</v>
@@ -1176,42 +1185,42 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L13">
         <v>1.5</v>
@@ -1223,7 +1232,7 @@
         <v>1.5</v>
       </c>
       <c r="O13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1233,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C3:X41"/>
+  <dimension ref="C3:X43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1255,7 +1264,7 @@
   <sheetData>
     <row r="3" spans="3:24" x14ac:dyDescent="0.45">
       <c r="L3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.45">
@@ -1263,10 +1272,10 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
         <v>21</v>
@@ -1289,13 +1298,13 @@
         <v>5</v>
       </c>
       <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
         <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="3:24" x14ac:dyDescent="0.45">
@@ -1303,19 +1312,19 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G6" s="1">
         <v>8.76</v>
       </c>
       <c r="L6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.45">
@@ -1323,19 +1332,19 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7">
         <v>25</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.45">
@@ -1343,7 +1352,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -1365,29 +1374,38 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G10">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="1">
+        <v>8.76</v>
+      </c>
       <c r="P11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="3:24" x14ac:dyDescent="0.45">
       <c r="P12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="T12" t="s">
         <v>21</v>
@@ -1398,7 +1416,7 @@
         <v>4</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q13" s="2">
         <v>2700</v>
@@ -1414,7 +1432,7 @@
         <v>EN[_]Hydro*</v>
       </c>
       <c r="W13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X13" t="s">
         <v>19</v>
@@ -1437,7 +1455,7 @@
         <v>5</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q14" s="2">
         <v>1110</v>
@@ -1453,10 +1471,10 @@
         <v>E[_]SPV*</v>
       </c>
       <c r="W14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="3:24" x14ac:dyDescent="0.45">
@@ -1467,7 +1485,7 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1476,7 +1494,7 @@
         <v>3</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q15" s="2">
         <v>4060</v>
@@ -1492,10 +1510,10 @@
         <v>E[_]WOF*</v>
       </c>
       <c r="W15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="X15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="3:24" x14ac:dyDescent="0.45">
@@ -1503,13 +1521,13 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G16" s="1">
         <v>8.76</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q16" s="2">
         <v>1500</v>
@@ -1525,10 +1543,10 @@
         <v>E[_]WON*</v>
       </c>
       <c r="W16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="3:24" x14ac:dyDescent="0.45">
@@ -1536,13 +1554,13 @@
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G17">
         <v>4</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q17" s="2">
         <v>70</v>
@@ -1571,13 +1589,13 @@
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q18" s="2">
         <v>16</v>
@@ -1606,13 +1624,13 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G19">
         <v>30</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q19" s="2">
         <v>120</v>
@@ -1641,13 +1659,13 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q20" s="2">
         <v>38</v>
@@ -1682,7 +1700,7 @@
         <v>0.25</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q21" s="2">
         <v>4</v>
@@ -1711,13 +1729,13 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G22">
         <v>20</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q22" s="2">
         <v>1.5</v>
@@ -1743,7 +1761,7 @@
     </row>
     <row r="23" spans="3:24" x14ac:dyDescent="0.45">
       <c r="P23" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q23" s="2">
         <v>3</v>
@@ -1769,7 +1787,7 @@
     </row>
     <row r="24" spans="3:24" x14ac:dyDescent="0.45">
       <c r="P24" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q24" s="2">
         <v>1.5</v>
@@ -1828,7 +1846,7 @@
     </row>
     <row r="30" spans="3:24" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -1916,10 +1934,10 @@
         <v>14</v>
       </c>
       <c r="D40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" t="s">
         <v>24</v>
-      </c>
-      <c r="E40" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.45">
@@ -1927,10 +1945,32 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="E41" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>